<commit_message>
Update edited session - 2025-11-20T11:55:48.292Z - Cache Bust ID: 1763639748292auif45tys
</commit_message>
<xml_diff>
--- a/log_history/Y3_B2526_Physiology_scanner1763638907179_5e3a997dbba4d784fa74ddee802563ced5b571682c1430f240639c3e60172369.xlsx
+++ b/log_history/Y3_B2526_Physiology_scanner1763638907179_5e3a997dbba4d784fa74ddee802563ced5b571682c1430f240639c3e60172369.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Physiology" sheetId="1" r:id="rId1"/>
+    <sheet name="Session" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -724,7 +724,7 @@
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>231521</v>
+        <v>231479</v>
       </c>
       <c r="B17" t="str">
         <v>Physiology</v>
@@ -733,7 +733,7 @@
         <v>20/11/2025</v>
       </c>
       <c r="D17" t="str">
-        <v>13:42:32</v>
+        <v>13:42:35</v>
       </c>
       <c r="E17" t="str">
         <v>Scan</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>231479</v>
+        <v>231450</v>
       </c>
       <c r="B18" t="str">
         <v>Physiology</v>
@@ -753,7 +753,7 @@
         <v>20/11/2025</v>
       </c>
       <c r="D18" t="str">
-        <v>13:42:35</v>
+        <v>13:42:38</v>
       </c>
       <c r="E18" t="str">
         <v>Scan</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>231450</v>
+        <v>231443</v>
       </c>
       <c r="B19" t="str">
         <v>Physiology</v>
@@ -773,7 +773,7 @@
         <v>20/11/2025</v>
       </c>
       <c r="D19" t="str">
-        <v>13:42:38</v>
+        <v>13:42:42</v>
       </c>
       <c r="E19" t="str">
         <v>Scan</v>
@@ -784,7 +784,7 @@
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>231443</v>
+        <v>231448</v>
       </c>
       <c r="B20" t="str">
         <v>Physiology</v>
@@ -793,7 +793,7 @@
         <v>20/11/2025</v>
       </c>
       <c r="D20" t="str">
-        <v>13:42:42</v>
+        <v>13:42:45</v>
       </c>
       <c r="E20" t="str">
         <v>Scan</v>
@@ -804,7 +804,7 @@
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>231448</v>
+        <v>231455</v>
       </c>
       <c r="B21" t="str">
         <v>Physiology</v>
@@ -813,7 +813,7 @@
         <v>20/11/2025</v>
       </c>
       <c r="D21" t="str">
-        <v>13:42:45</v>
+        <v>13:42:48</v>
       </c>
       <c r="E21" t="str">
         <v>Scan</v>
@@ -824,7 +824,7 @@
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>231455</v>
+        <v>231432</v>
       </c>
       <c r="B22" t="str">
         <v>Physiology</v>
@@ -833,10 +833,10 @@
         <v>20/11/2025</v>
       </c>
       <c r="D22" t="str">
-        <v>13:42:48</v>
+        <v>13:43:02</v>
       </c>
       <c r="E22" t="str">
-        <v>Scan</v>
+        <v>Manual</v>
       </c>
       <c r="F22" t="str">
         <v>neveen.nashaat@med.asu.edu.eg</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>231432</v>
+        <v>231444</v>
       </c>
       <c r="B23" t="str">
         <v>Physiology</v>
@@ -853,38 +853,18 @@
         <v>20/11/2025</v>
       </c>
       <c r="D23" t="str">
-        <v>13:43:02</v>
+        <v>13:43:11</v>
       </c>
       <c r="E23" t="str">
-        <v>Manual</v>
+        <v>Scan</v>
       </c>
       <c r="F23" t="str">
-        <v>neveen.nashaat@med.asu.edu.eg</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="str">
-        <v>231444</v>
-      </c>
-      <c r="B24" t="str">
-        <v>Physiology</v>
-      </c>
-      <c r="C24" t="str">
-        <v>20/11/2025</v>
-      </c>
-      <c r="D24" t="str">
-        <v>13:43:11</v>
-      </c>
-      <c r="E24" t="str">
-        <v>Scan</v>
-      </c>
-      <c r="F24" t="str">
         <v>neveen.nashaat@med.asu.edu.eg</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F24"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F23"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>